<commit_message>
Updated all in one format
</commit_message>
<xml_diff>
--- a/Master Template.xlsx
+++ b/Master Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TOPMATT\Documents\Bet9ja Excel Macro\Bet9ja_Excel_Macro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51EED5B5-6566-4BB7-BE0B-0D6B3EB9F687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8782BF4E-95F1-4A7E-8ECB-9E4574790A2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2740,6 +2740,7 @@
     <sheetNames>
       <sheetName val="MASTER"/>
       <sheetName val="Season 12684"/>
+      <sheetName val="Sheet1"/>
       <sheetName val="Season 12722"/>
       <sheetName val="Season 12729"/>
       <sheetName val="Season 12736"/>
@@ -3041,6 +3042,7 @@
       <sheetData sheetId="142"/>
       <sheetData sheetId="143"/>
       <sheetData sheetId="144"/>
+      <sheetData sheetId="145"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3312,8 +3314,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="BL21:CS52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BR16" workbookViewId="0">
-      <selection activeCell="BL21" sqref="BL21:CS52"/>
+    <sheetView tabSelected="1" topLeftCell="AN16" workbookViewId="0">
+      <selection activeCell="BM23" sqref="BM23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>